<commit_message>
descw-1280 finalize report template
* fix query for missing scope column
* adjust styling
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_3_rpt_CA_AmendmentTypes-FY-Summary.xlsx
+++ b/backend/reports/xlsx/Tab_3_rpt_CA_AmendmentTypes-FY-Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7FEBBF-A5C0-9143-8AA3-28F50AA1FC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B7293F-08E2-C14D-BCA7-229ACC2EDAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
-    <t>Active Contractor Resource List</t>
-  </si>
-  <si>
     <t>FY</t>
   </si>
   <si>
@@ -76,12 +73,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>{#row=d.report[i].projects[i]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {#rows=d.report[i].projects[i+1]}</t>
-  </si>
-  <si>
     <t xml:space="preserve"> {$row.fiscal_year}</t>
   </si>
   <si>
@@ -116,6 +107,15 @@
   </si>
   <si>
     <t>{$row.end_date}</t>
+  </si>
+  <si>
+    <t>{#row=d.report[i]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {#rows=d.report[i+1]}</t>
+  </si>
+  <si>
+    <t>Contract Amendment Stats by Type</t>
   </si>
 </sst>
 </file>
@@ -125,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,6 +138,11 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
+      <b/>
+      <sz val="9"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
       <sz val="8.5"/>
       <name val="BCSans-Regular"/>
     </font>
@@ -147,16 +152,27 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="BCSans-Regular"/>
     </font>
   </fonts>
   <fills count="4">
@@ -179,7 +195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -261,65 +277,49 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,15 +349,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1385845</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>308163</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>680356</xdr:rowOff>
+      <xdr:rowOff>468656</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -386,8 +386,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2411614" cy="680356"/>
+          <a:off x="1" y="0"/>
+          <a:ext cx="1662206" cy="468656"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -701,152 +701,152 @@
   </sheetPr>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K4" sqref="A3:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="41" customHeight="1" thickBot="1">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="33" thickBot="1">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="35" thickBot="1">
-      <c r="A2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="12" t="s">
         <v>10</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="E3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="F3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="G3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="H3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="I3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="J3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="13" t="s">
         <v>21</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="A4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" ht="19">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" s="16" customFormat="1" ht="11">
-      <c r="B6" s="16" t="s">
-        <v>12</v>
+    <row r="6" spans="1:11" s="6" customFormat="1" ht="19">
+      <c r="B6" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="B7" s="16" t="s">
-        <v>13</v>
+    <row r="7" spans="1:11" ht="19">
+      <c r="B7" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>